<commit_message>
Added data on multiple hidden layers
</commit_message>
<xml_diff>
--- a/Code/Neural Networks/SineApproximator_Loss_Function_Data.xlsx
+++ b/Code/Neural Networks/SineApproximator_Loss_Function_Data.xlsx
@@ -5,13 +5,17 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Vary_Training_Points" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Vary_Iteration" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Vary_Training_Points_Graph" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Vary_Training_Points" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Multiple_Hidden_Layers_Graph" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Multiple_Hidden_Layers" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Vary_Iteration_Graph" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Vary_Iteration" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="24">
   <si>
     <t xml:space="preserve">Hidden Dimension Value</t>
   </si>
@@ -71,6 +75,12 @@
     <t xml:space="preserve">Loss for 100,000 Training Points (3000 Iterations)</t>
   </si>
   <si>
+    <t xml:space="preserve">Number of Hidden Layers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loss Function After 3,000 Iterations</t>
+  </si>
+  <si>
     <t xml:space="preserve">Loss After 5000 iterations (10,000 training points)</t>
   </si>
   <si>
@@ -96,7 +106,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -119,6 +129,30 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b val="true"/>
       <u val="single"/>
       <sz val="10"/>
@@ -134,18 +168,21 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="13"/>
-      <name val="Arial"/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Arial"/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -196,15 +233,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -235,14 +272,14 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF5B9BD5"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFD9D9D9"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -280,7 +317,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -360,6 +397,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -467,6 +505,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -574,6 +613,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -681,6 +721,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -756,11 +797,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="73235619"/>
-        <c:axId val="26822604"/>
+        <c:axId val="68913804"/>
+        <c:axId val="87262798"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73235619"/>
+        <c:axId val="68913804"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -804,15 +845,16 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="6480">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
+            <a:round/>
           </a:ln>
         </c:spPr>
         <c:txPr>
@@ -833,12 +875,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26822604"/>
+        <c:crossAx val="87262798"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="26822604"/>
+        <c:axId val="87262798"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -882,15 +924,16 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="6480">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
+            <a:round/>
           </a:ln>
         </c:spPr>
         <c:txPr>
@@ -911,7 +954,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73235619"/>
+        <c:crossAx val="68913804"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -948,7 +991,310 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1800" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1800" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>3,000 Iterations, 10,000 Training Points, 50 Neurons in Hidden Layer</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="19080">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="13"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="5b9bd5"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Multiple_Hidden_Layers!$A$2:$A$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Multiple_Hidden_Layers!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.003889</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.001484</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.000296</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="64707423"/>
+        <c:axId val="82391704"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="64707423"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1600" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1600" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Number of Hidden Layers</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="25560">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1100" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="82391704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="82391704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1600" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1600" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Value of Loss Function  for One Run</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="25560">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1100" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64707423"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="28440">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1028,6 +1374,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1135,6 +1482,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1242,6 +1590,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1317,11 +1666,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="19439128"/>
-        <c:axId val="17850749"/>
+        <c:axId val="96210497"/>
+        <c:axId val="5632748"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="19439128"/>
+        <c:axId val="96210497"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1365,15 +1714,16 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="6480">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
+            <a:round/>
           </a:ln>
         </c:spPr>
         <c:txPr>
@@ -1394,12 +1744,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17850749"/>
+        <c:crossAx val="5632748"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="17850749"/>
+        <c:axId val="5632748"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1443,15 +1793,16 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="6480">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
+            <a:round/>
           </a:ln>
         </c:spPr>
         <c:txPr>
@@ -1472,7 +1823,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19439128"/>
+        <c:crossAx val="96210497"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1513,25 +1864,25 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>188640</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>11160</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>618120</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>162360</xdr:rowOff>
+      <xdr:colOff>9360</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>113760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvPr id="0" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8105040" y="11160"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="8668080" cy="6291000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1548,25 +1899,60 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>288360</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>90360</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>717840</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>78840</xdr:rowOff>
+      <xdr:colOff>9360</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>113760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvPr id="1" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8204760" y="415440"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="8668080" cy="6291000"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>9360</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>113760</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="8668080" cy="6291000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1582,1073 +1968,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L32" activeCellId="0" sqref="L32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="119" zoomScaleNormal="119" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A5:B5 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.0663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="12.5918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.76530612244898"/>
   </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>0.45521</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>0.46374</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>0.475828</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>0.481189</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>0.479303</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <f aca="false">AVERAGE(B3:F3)</f>
-        <v>0.471054</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <f aca="false">STDEV(B3:F3)</f>
-        <v>0.011158878012596</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>0.25607</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>0.308449</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>0.311423</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>0.318015</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>0.271953</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <f aca="false">AVERAGE(B4:F4)</f>
-        <v>0.293182</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <f aca="false">STDEV(B4:F4)</f>
-        <v>0.0274338488185672</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>0.314604</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>0.450731</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>0.088501</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>0.310546</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>0.170506</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <f aca="false">AVERAGE(B5:F5)</f>
-        <v>0.2669776</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <f aca="false">STDEV(B5:F5)</f>
-        <v>0.140616906719285</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>0.04131</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>0.09453</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>0.085227</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>0.090565</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>0.088506</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <f aca="false">AVERAGE(B6:F6)</f>
-        <v>0.0800276</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <f aca="false">STDEV(B6:F6)</f>
-        <v>0.0219050563865971</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>0.002863</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>0.00507</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>0.001474</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>0.001568</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>0.001412</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <f aca="false">AVERAGE(B7:F7)</f>
-        <v>0.0024774</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <f aca="false">STDEV(B7:F7)</f>
-        <v>0.00156837170339177</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>250</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>0.006826</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>0.008096</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>0.002523</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>0.00125</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>0.003604</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <f aca="false">AVERAGE(B8:F8)</f>
-        <v>0.0044598</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <f aca="false">STDEV(B8:F8)</f>
-        <v>0.00289858831157514</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>0.003908</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>0.000582</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>0.000893</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>0.003777</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>0.005086</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <f aca="false">AVERAGE(B9:F9)</f>
-        <v>0.0028492</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <f aca="false">STDEV(B9:F9)</f>
-        <v>0.0019970014271402</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>0.014241</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>0.007949</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>0.006162</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>0.001319</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>0.000384</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <f aca="false">AVERAGE(B10:F10)</f>
-        <v>0.006011</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <f aca="false">STDEV(B10:F10)</f>
-        <v>0.00559440653689022</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>0.463689</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>0.464652</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>0.469117</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>0.467187</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>0.460454</v>
-      </c>
-      <c r="G14" s="0" t="n">
-        <f aca="false">AVERAGE(B14:F14)</f>
-        <v>0.4650198</v>
-      </c>
-      <c r="H14" s="0" t="n">
-        <f aca="false">STDEV(B14:F14)</f>
-        <v>0.00332553149135594</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>0.438998</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>0.305529</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>0.447328</v>
-      </c>
-      <c r="E15" s="0" t="n">
-        <v>0.364528</v>
-      </c>
-      <c r="F15" s="0" t="n">
-        <v>0.444103</v>
-      </c>
-      <c r="G15" s="0" t="n">
-        <f aca="false">AVERAGE(B15:F15)</f>
-        <v>0.4000972</v>
-      </c>
-      <c r="H15" s="0" t="n">
-        <f aca="false">STDEV(B15:F15)</f>
-        <v>0.0630254781473334</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>0.034906</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>0.315709</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>0.304165</v>
-      </c>
-      <c r="E16" s="0" t="n">
-        <v>0.00569</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <v>0.006483</v>
-      </c>
-      <c r="G16" s="0" t="n">
-        <f aca="false">AVERAGE(B16:F16)</f>
-        <v>0.1333906</v>
-      </c>
-      <c r="H16" s="0" t="n">
-        <f aca="false">STDEV(B16:F16)</f>
-        <v>0.161644744183967</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>0.175448</v>
-      </c>
-      <c r="C17" s="0" t="n">
-        <v>0.090968</v>
-      </c>
-      <c r="D17" s="0" t="n">
-        <v>0.093626</v>
-      </c>
-      <c r="E17" s="0" t="n">
-        <v>0.086604</v>
-      </c>
-      <c r="F17" s="0" t="n">
-        <v>0.010062</v>
-      </c>
-      <c r="G17" s="0" t="n">
-        <f aca="false">AVERAGE(B17:F17)</f>
-        <v>0.0913416</v>
-      </c>
-      <c r="H17" s="0" t="n">
-        <f aca="false">STDEV(B17:F17)</f>
-        <v>0.0585407183317731</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="B18" s="0" t="n">
-        <v>0.002849</v>
-      </c>
-      <c r="C18" s="0" t="n">
-        <v>0.006384</v>
-      </c>
-      <c r="D18" s="0" t="n">
-        <v>0.004563</v>
-      </c>
-      <c r="E18" s="0" t="n">
-        <v>0.002226</v>
-      </c>
-      <c r="F18" s="0" t="n">
-        <v>0.004213</v>
-      </c>
-      <c r="G18" s="0" t="n">
-        <f aca="false">AVERAGE(B18:F18)</f>
-        <v>0.004047</v>
-      </c>
-      <c r="H18" s="0" t="n">
-        <f aca="false">STDEV(B18:F18)</f>
-        <v>0.00162069630097684</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
-        <v>250</v>
-      </c>
-      <c r="B19" s="0" t="n">
-        <v>0.004159</v>
-      </c>
-      <c r="C19" s="0" t="n">
-        <v>0.001595</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <v>0.00357</v>
-      </c>
-      <c r="E19" s="0" t="n">
-        <v>0.002232</v>
-      </c>
-      <c r="F19" s="0" t="n">
-        <v>0.010177</v>
-      </c>
-      <c r="G19" s="0" t="n">
-        <f aca="false">AVERAGE(B19:F19)</f>
-        <v>0.0043466</v>
-      </c>
-      <c r="H19" s="0" t="n">
-        <f aca="false">STDEV(B19:F19)</f>
-        <v>0.00341594427647759</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="B20" s="0" t="n">
-        <v>0.002904</v>
-      </c>
-      <c r="C20" s="0" t="n">
-        <v>0.000737</v>
-      </c>
-      <c r="D20" s="0" t="n">
-        <v>0.001833</v>
-      </c>
-      <c r="E20" s="0" t="n">
-        <v>0.004316</v>
-      </c>
-      <c r="F20" s="0" t="n">
-        <v>0.003296</v>
-      </c>
-      <c r="G20" s="0" t="n">
-        <f aca="false">AVERAGE(B20:F20)</f>
-        <v>0.0026172</v>
-      </c>
-      <c r="H20" s="0" t="n">
-        <f aca="false">STDEV(B20:F20)</f>
-        <v>0.00137650524880946</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="B21" s="0" t="n">
-        <v>0.002479</v>
-      </c>
-      <c r="C21" s="0" t="n">
-        <v>0.001289</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="E21" s="0" t="n">
-        <v>0.005219</v>
-      </c>
-      <c r="F21" s="0" t="n">
-        <v>0.000789</v>
-      </c>
-      <c r="G21" s="0" t="n">
-        <f aca="false">AVERAGE(B21:F21)</f>
-        <v>0.0023552</v>
-      </c>
-      <c r="H21" s="0" t="n">
-        <f aca="false">STDEV(B21:F21)</f>
-        <v>0.00172718041906455</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K24" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B25" s="0" t="n">
-        <v>0.469294</v>
-      </c>
-      <c r="C25" s="0" t="n">
-        <v>0.467821</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <v>0.463247</v>
-      </c>
-      <c r="E25" s="0" t="n">
-        <v>0.466117</v>
-      </c>
-      <c r="F25" s="0" t="n">
-        <v>0.469118</v>
-      </c>
-      <c r="G25" s="0" t="n">
-        <f aca="false">AVERAGE(B25:F25)</f>
-        <v>0.4671194</v>
-      </c>
-      <c r="H25" s="0" t="n">
-        <f aca="false">STDEV(B25:F25)</f>
-        <v>0.00251076767145031</v>
-      </c>
-      <c r="K25" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B26" s="0" t="n">
-        <v>0.30836</v>
-      </c>
-      <c r="C26" s="0" t="n">
-        <v>0.430063</v>
-      </c>
-      <c r="D26" s="0" t="n">
-        <v>0.308547</v>
-      </c>
-      <c r="E26" s="0" t="n">
-        <v>0.313782</v>
-      </c>
-      <c r="F26" s="0" t="n">
-        <v>0.441661</v>
-      </c>
-      <c r="G26" s="0" t="n">
-        <f aca="false">AVERAGE(B26:F26)</f>
-        <v>0.3604826</v>
-      </c>
-      <c r="H26" s="0" t="n">
-        <f aca="false">STDEV(B26:F26)</f>
-        <v>0.0689680772336013</v>
-      </c>
-      <c r="K26" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="B27" s="0" t="n">
-        <v>0.091637</v>
-      </c>
-      <c r="C27" s="0" t="n">
-        <v>0.09211</v>
-      </c>
-      <c r="D27" s="0" t="n">
-        <v>0.004548</v>
-      </c>
-      <c r="E27" s="0" t="n">
-        <v>0.090334</v>
-      </c>
-      <c r="F27" s="0" t="n">
-        <v>0.004551</v>
-      </c>
-      <c r="G27" s="0" t="n">
-        <f aca="false">AVERAGE(B27:F27)</f>
-        <v>0.056636</v>
-      </c>
-      <c r="H27" s="0" t="n">
-        <f aca="false">STDEV(B27:F27)</f>
-        <v>0.0475526993187558</v>
-      </c>
-      <c r="K27" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="B28" s="0" t="n">
-        <v>0.22522</v>
-      </c>
-      <c r="C28" s="0" t="n">
-        <v>0.18132</v>
-      </c>
-      <c r="D28" s="0" t="n">
-        <v>0.182611</v>
-      </c>
-      <c r="E28" s="0" t="n">
-        <v>0.107289</v>
-      </c>
-      <c r="F28" s="0" t="n">
-        <v>0.003607</v>
-      </c>
-      <c r="G28" s="0" t="n">
-        <f aca="false">AVERAGE(B28:F28)</f>
-        <v>0.1400094</v>
-      </c>
-      <c r="H28" s="0" t="n">
-        <f aca="false">STDEV(B28:F28)</f>
-        <v>0.0872618869398319</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="B29" s="0" t="n">
-        <v>0.003692</v>
-      </c>
-      <c r="C29" s="0" t="n">
-        <v>0.008182</v>
-      </c>
-      <c r="D29" s="0" t="n">
-        <v>0.002554</v>
-      </c>
-      <c r="E29" s="0" t="n">
-        <v>0.0019</v>
-      </c>
-      <c r="F29" s="0" t="n">
-        <v>0.000916</v>
-      </c>
-      <c r="G29" s="0" t="n">
-        <f aca="false">AVERAGE(B29:F29)</f>
-        <v>0.0034488</v>
-      </c>
-      <c r="H29" s="0" t="n">
-        <f aca="false">STDEV(B29:F29)</f>
-        <v>0.00283182153392476</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
-        <v>250</v>
-      </c>
-      <c r="B30" s="0" t="n">
-        <v>0.006043</v>
-      </c>
-      <c r="C30" s="0" t="n">
-        <v>0.003379</v>
-      </c>
-      <c r="D30" s="0" t="n">
-        <v>0.002006</v>
-      </c>
-      <c r="E30" s="0" t="n">
-        <v>0.000341</v>
-      </c>
-      <c r="F30" s="0" t="n">
-        <v>0.0016</v>
-      </c>
-      <c r="G30" s="0" t="n">
-        <f aca="false">AVERAGE(B30:F30)</f>
-        <v>0.0026738</v>
-      </c>
-      <c r="H30" s="0" t="n">
-        <f aca="false">STDEV(B30:F30)</f>
-        <v>0.00217311842751379</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="B31" s="0" t="n">
-        <v>0.033083</v>
-      </c>
-      <c r="C31" s="0" t="n">
-        <v>0.007218</v>
-      </c>
-      <c r="D31" s="0" t="n">
-        <v>0.03983</v>
-      </c>
-      <c r="E31" s="0" t="n">
-        <v>0.00136</v>
-      </c>
-      <c r="F31" s="0" t="n">
-        <v>0.017548</v>
-      </c>
-      <c r="G31" s="0" t="n">
-        <f aca="false">AVERAGE(B31:F31)</f>
-        <v>0.0198078</v>
-      </c>
-      <c r="H31" s="0" t="n">
-        <f aca="false">STDEV(B31:F31)</f>
-        <v>0.0164396663043992</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="B32" s="0" t="n">
-        <v>0.002524</v>
-      </c>
-      <c r="C32" s="0" t="n">
-        <v>0.001158</v>
-      </c>
-      <c r="D32" s="0" t="n">
-        <v>0.008493</v>
-      </c>
-      <c r="E32" s="0" t="n">
-        <v>0.001545</v>
-      </c>
-      <c r="F32" s="0" t="n">
-        <v>0.001028</v>
-      </c>
-      <c r="G32" s="0" t="n">
-        <f aca="false">AVERAGE(B32:F32)</f>
-        <v>0.0029496</v>
-      </c>
-      <c r="H32" s="0" t="n">
-        <f aca="false">STDEV(B32:F32)</f>
-        <v>0.00315379522163377</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B37" s="0" t="n">
-        <v>0.465324</v>
-      </c>
-      <c r="C37" s="0" t="n">
-        <v>0.466957</v>
-      </c>
-      <c r="D37" s="0" t="n">
-        <v>0.467213</v>
-      </c>
-      <c r="E37" s="0" t="n">
-        <v>0.466626</v>
-      </c>
-      <c r="F37" s="0" t="n">
-        <v>0.465238</v>
-      </c>
-      <c r="G37" s="0" t="n">
-        <f aca="false">AVERAGE(B37:F37)</f>
-        <v>0.4662716</v>
-      </c>
-      <c r="H37" s="0" t="n">
-        <f aca="false">STDEV(B37:F37)</f>
-        <v>0.000928423556357767</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B38" s="0" t="n">
-        <v>0.442109</v>
-      </c>
-      <c r="C38" s="0" t="n">
-        <v>0.259074</v>
-      </c>
-      <c r="D38" s="0" t="n">
-        <v>0.310232</v>
-      </c>
-      <c r="E38" s="0" t="n">
-        <v>0.092753</v>
-      </c>
-      <c r="F38" s="0" t="n">
-        <v>0.447128</v>
-      </c>
-      <c r="G38" s="0" t="n">
-        <f aca="false">AVERAGE(B38:F38)</f>
-        <v>0.3102592</v>
-      </c>
-      <c r="H38" s="0" t="n">
-        <f aca="false">STDEV(B38:F38)</f>
-        <v>0.146668257174823</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="B39" s="0" t="n">
-        <v>0.179828</v>
-      </c>
-      <c r="C39" s="0" t="n">
-        <v>0.177575</v>
-      </c>
-      <c r="D39" s="0" t="n">
-        <v>0.091855</v>
-      </c>
-      <c r="E39" s="0" t="n">
-        <v>0.011167</v>
-      </c>
-      <c r="F39" s="0" t="n">
-        <v>0.180568</v>
-      </c>
-      <c r="G39" s="0" t="n">
-        <f aca="false">AVERAGE(B39:F39)</f>
-        <v>0.1281986</v>
-      </c>
-      <c r="H39" s="0" t="n">
-        <f aca="false">STDEV(B39:F39)</f>
-        <v>0.0756032911605044</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="B40" s="0" t="n">
-        <v>0.011642</v>
-      </c>
-      <c r="C40" s="0" t="n">
-        <v>0.042119</v>
-      </c>
-      <c r="D40" s="0" t="n">
-        <v>0.091441</v>
-      </c>
-      <c r="E40" s="0" t="n">
-        <v>0.002989</v>
-      </c>
-      <c r="F40" s="0" t="n">
-        <v>0.180346</v>
-      </c>
-      <c r="G40" s="0" t="n">
-        <f aca="false">AVERAGE(B40:F40)</f>
-        <v>0.0657074</v>
-      </c>
-      <c r="H40" s="0" t="n">
-        <f aca="false">STDEV(B40:F40)</f>
-        <v>0.072830804899438</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="B41" s="0" t="n">
-        <v>0.001895</v>
-      </c>
-      <c r="C41" s="0" t="n">
-        <v>0.001713</v>
-      </c>
-      <c r="D41" s="0" t="n">
-        <v>0.001549</v>
-      </c>
-      <c r="E41" s="0" t="n">
-        <v>0.004337</v>
-      </c>
-      <c r="F41" s="0" t="n">
-        <v>0.002444</v>
-      </c>
-      <c r="G41" s="0" t="n">
-        <f aca="false">AVERAGE(B41:F41)</f>
-        <v>0.0023876</v>
-      </c>
-      <c r="H41" s="0" t="n">
-        <f aca="false">STDEV(B41:F41)</f>
-        <v>0.00114065016547581</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
-        <v>250</v>
-      </c>
-      <c r="B42" s="0" t="n">
-        <v>0.00553</v>
-      </c>
-      <c r="C42" s="0" t="n">
-        <v>0.00196</v>
-      </c>
-      <c r="D42" s="0" t="n">
-        <v>0.003312</v>
-      </c>
-      <c r="E42" s="0" t="n">
-        <v>0.004414</v>
-      </c>
-      <c r="F42" s="0" t="n">
-        <v>0.054637</v>
-      </c>
-      <c r="G42" s="0" t="n">
-        <f aca="false">AVERAGE(B42:F42)</f>
-        <v>0.0139706</v>
-      </c>
-      <c r="H42" s="0" t="n">
-        <f aca="false">STDEV(B42:F42)</f>
-        <v>0.0227716308550793</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="B43" s="0" t="n">
-        <v>0.004197</v>
-      </c>
-      <c r="C43" s="0" t="n">
-        <v>0.005984</v>
-      </c>
-      <c r="D43" s="0" t="n">
-        <v>0.004891</v>
-      </c>
-      <c r="E43" s="0" t="n">
-        <v>0.006827</v>
-      </c>
-      <c r="F43" s="0" t="n">
-        <v>0.004754</v>
-      </c>
-      <c r="G43" s="0" t="n">
-        <f aca="false">AVERAGE(B43:F43)</f>
-        <v>0.0053306</v>
-      </c>
-      <c r="H43" s="0" t="n">
-        <f aca="false">STDEV(B43:F43)</f>
-        <v>0.00105793539500293</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="B44" s="0" t="n">
-        <v>0.002056</v>
-      </c>
-      <c r="C44" s="0" t="n">
-        <v>0.000552</v>
-      </c>
-      <c r="D44" s="0" t="n">
-        <v>0.001004</v>
-      </c>
-      <c r="E44" s="0" t="n">
-        <v>0.000366</v>
-      </c>
-      <c r="F44" s="0" t="n">
-        <v>0.000564</v>
-      </c>
-      <c r="G44" s="0" t="n">
-        <f aca="false">AVERAGE(B44:F44)</f>
-        <v>0.0009084</v>
-      </c>
-      <c r="H44" s="0" t="n">
-        <f aca="false">STDEV(B44:F44)</f>
-        <v>0.0006829998535871</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B35:F35"/>
-  </mergeCells>
+  <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="75" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2659,31 +1997,1221 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J35" activeCellId="0" sqref="J35"/>
+      <selection pane="topLeft" activeCell="L32" activeCellId="1" sqref="A5:B5 L32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="12.9591836734694"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.45521</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.46374</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0.475828</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0.481189</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0.479303</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">AVERAGE(B3:F3)</f>
+        <v>0.471054</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <f aca="false">STDEV(B3:F3)</f>
+        <v>0.0111588780125961</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.25607</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.308449</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0.311423</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0.318015</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0.271953</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <f aca="false">AVERAGE(B4:F4)</f>
+        <v>0.293182</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <f aca="false">STDEV(B4:F4)</f>
+        <v>0.0274338488185672</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.314604</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.450731</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0.088501</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0.310546</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0.170506</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">AVERAGE(B5:F5)</f>
+        <v>0.2669776</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <f aca="false">STDEV(B5:F5)</f>
+        <v>0.140616906719285</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.04131</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.09453</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0.085227</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0.090565</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0.088506</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">AVERAGE(B6:F6)</f>
+        <v>0.0800276</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <f aca="false">STDEV(B6:F6)</f>
+        <v>0.0219050563865971</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.002863</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.00507</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0.001474</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0.001568</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0.001412</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <f aca="false">AVERAGE(B7:F7)</f>
+        <v>0.0024774</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <f aca="false">STDEV(B7:F7)</f>
+        <v>0.00156837170339177</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.006826</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.008096</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0.002523</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0.00125</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>0.003604</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <f aca="false">AVERAGE(B8:F8)</f>
+        <v>0.0044598</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <f aca="false">STDEV(B8:F8)</f>
+        <v>0.00289858831157514</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.003908</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0.000582</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0.000893</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0.003777</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0.005086</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <f aca="false">AVERAGE(B9:F9)</f>
+        <v>0.0028492</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <f aca="false">STDEV(B9:F9)</f>
+        <v>0.0019970014271402</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.014241</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.007949</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0.006162</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0.001319</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>0.000384</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <f aca="false">AVERAGE(B10:F10)</f>
+        <v>0.006011</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <f aca="false">STDEV(B10:F10)</f>
+        <v>0.00559440653689022</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>0.463689</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0.464652</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>0.469117</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>0.467187</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>0.460454</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <f aca="false">AVERAGE(B14:F14)</f>
+        <v>0.4650198</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <f aca="false">STDEV(B14:F14)</f>
+        <v>0.00332553149135592</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>0.438998</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0.305529</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>0.447328</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>0.364528</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>0.444103</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <f aca="false">AVERAGE(B15:F15)</f>
+        <v>0.4000972</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <f aca="false">STDEV(B15:F15)</f>
+        <v>0.0630254781473334</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>0.034906</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0.315709</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>0.304165</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>0.00569</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>0.006483</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <f aca="false">AVERAGE(B16:F16)</f>
+        <v>0.1333906</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <f aca="false">STDEV(B16:F16)</f>
+        <v>0.161644744183967</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>0.175448</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0.090968</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>0.093626</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>0.086604</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>0.010062</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <f aca="false">AVERAGE(B17:F17)</f>
+        <v>0.0913416</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <f aca="false">STDEV(B17:F17)</f>
+        <v>0.0585407183317732</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>0.002849</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0.006384</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>0.004563</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>0.002226</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>0.004213</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <f aca="false">AVERAGE(B18:F18)</f>
+        <v>0.004047</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <f aca="false">STDEV(B18:F18)</f>
+        <v>0.00162069630097684</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0.004159</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0.001595</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>0.00357</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0.002232</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>0.010177</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <f aca="false">AVERAGE(B19:F19)</f>
+        <v>0.0043466</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <f aca="false">STDEV(B19:F19)</f>
+        <v>0.00341594427647759</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>0.002904</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>0.000737</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>0.001833</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>0.004316</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>0.003296</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <f aca="false">AVERAGE(B20:F20)</f>
+        <v>0.0026172</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <f aca="false">STDEV(B20:F20)</f>
+        <v>0.00137650524880946</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>0.002479</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>0.001289</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>0.005219</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>0.000789</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <f aca="false">AVERAGE(B21:F21)</f>
+        <v>0.0023552</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <f aca="false">STDEV(B21:F21)</f>
+        <v>0.00172718041906455</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K24" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>0.469294</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>0.467821</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>0.463247</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>0.466117</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>0.469118</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <f aca="false">AVERAGE(B25:F25)</f>
+        <v>0.4671194</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <f aca="false">STDEV(B25:F25)</f>
+        <v>0.00251076767145032</v>
+      </c>
+      <c r="K25" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>0.30836</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>0.430063</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>0.308547</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>0.313782</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>0.441661</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <f aca="false">AVERAGE(B26:F26)</f>
+        <v>0.3604826</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <f aca="false">STDEV(B26:F26)</f>
+        <v>0.0689680772336013</v>
+      </c>
+      <c r="K26" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>0.091637</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>0.09211</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>0.004548</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>0.090334</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>0.004551</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <f aca="false">AVERAGE(B27:F27)</f>
+        <v>0.056636</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <f aca="false">STDEV(B27:F27)</f>
+        <v>0.0475526993187558</v>
+      </c>
+      <c r="K27" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>0.22522</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>0.18132</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>0.182611</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>0.107289</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>0.003607</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <f aca="false">AVERAGE(B28:F28)</f>
+        <v>0.1400094</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <f aca="false">STDEV(B28:F28)</f>
+        <v>0.0872618869398319</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>0.003692</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>0.008182</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>0.002554</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>0.0019</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>0.000916</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <f aca="false">AVERAGE(B29:F29)</f>
+        <v>0.0034488</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <f aca="false">STDEV(B29:F29)</f>
+        <v>0.00283182153392476</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>0.006043</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>0.003379</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>0.002006</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>0.000341</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>0.0016</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <f aca="false">AVERAGE(B30:F30)</f>
+        <v>0.0026738</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <f aca="false">STDEV(B30:F30)</f>
+        <v>0.00217311842751379</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>0.033083</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>0.007218</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>0.03983</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>0.00136</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>0.017548</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <f aca="false">AVERAGE(B31:F31)</f>
+        <v>0.0198078</v>
+      </c>
+      <c r="H31" s="0" t="n">
+        <f aca="false">STDEV(B31:F31)</f>
+        <v>0.0164396663043992</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>0.002524</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>0.001158</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>0.008493</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>0.001545</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>0.001028</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <f aca="false">AVERAGE(B32:F32)</f>
+        <v>0.0029496</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <f aca="false">STDEV(B32:F32)</f>
+        <v>0.00315379522163377</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>0.465324</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>0.466957</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>0.467213</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>0.466626</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>0.465238</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <f aca="false">AVERAGE(B37:F37)</f>
+        <v>0.4662716</v>
+      </c>
+      <c r="H37" s="0" t="n">
+        <f aca="false">STDEV(B37:F37)</f>
+        <v>0.000928423556357767</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>0.442109</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>0.259074</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>0.310232</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>0.092753</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>0.447128</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <f aca="false">AVERAGE(B38:F38)</f>
+        <v>0.3102592</v>
+      </c>
+      <c r="H38" s="0" t="n">
+        <f aca="false">STDEV(B38:F38)</f>
+        <v>0.146668257174823</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>0.179828</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>0.177575</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>0.091855</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>0.011167</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>0.180568</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <f aca="false">AVERAGE(B39:F39)</f>
+        <v>0.1281986</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <f aca="false">STDEV(B39:F39)</f>
+        <v>0.0756032911605044</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>0.011642</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>0.042119</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>0.091441</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>0.002989</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>0.180346</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <f aca="false">AVERAGE(B40:F40)</f>
+        <v>0.0657074</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <f aca="false">STDEV(B40:F40)</f>
+        <v>0.072830804899438</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>0.001895</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>0.001713</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>0.001549</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>0.004337</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>0.002444</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <f aca="false">AVERAGE(B41:F41)</f>
+        <v>0.0023876</v>
+      </c>
+      <c r="H41" s="0" t="n">
+        <f aca="false">STDEV(B41:F41)</f>
+        <v>0.00114065016547581</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>0.00553</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>0.00196</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>0.003312</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>0.004414</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>0.054637</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <f aca="false">AVERAGE(B42:F42)</f>
+        <v>0.0139706</v>
+      </c>
+      <c r="H42" s="0" t="n">
+        <f aca="false">STDEV(B42:F42)</f>
+        <v>0.0227716308550793</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>0.004197</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>0.005984</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>0.004891</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>0.006827</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>0.004754</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <f aca="false">AVERAGE(B43:F43)</f>
+        <v>0.0053306</v>
+      </c>
+      <c r="H43" s="0" t="n">
+        <f aca="false">STDEV(B43:F43)</f>
+        <v>0.00105793539500293</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>0.002056</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>0.000552</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>0.001004</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>0.000366</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>0.000564</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <f aca="false">AVERAGE(B44:F44)</f>
+        <v>0.0009084</v>
+      </c>
+      <c r="H44" s="0" t="n">
+        <f aca="false">STDEV(B44:F44)</f>
+        <v>0.0006829998535871</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B35:F35"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="true"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="119" zoomScaleNormal="119" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A5:B5 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.0663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="12.5918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.76530612244898"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="75" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.5510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.9387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.89285714285714"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.003889</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.001484</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.000296</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="true"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="119" zoomScaleNormal="119" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A5:B5 A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.76530612244898"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="75" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H38"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="1" sqref="A5:B5 I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="12.9591836734694"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>2</v>
@@ -2707,7 +3235,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
@@ -2735,7 +3263,7 @@
         <v>0.00545803744948676</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>10</v>
       </c>
@@ -2763,7 +3291,7 @@
         <v>0.0936395306523906</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>50</v>
       </c>
@@ -2791,7 +3319,7 @@
         <v>0.013882872170412</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>100</v>
       </c>
@@ -2819,7 +3347,7 @@
         <v>0.0020956117961111</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>200</v>
       </c>
@@ -2847,7 +3375,7 @@
         <v>0.00132611417306354</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>250</v>
       </c>
@@ -2875,7 +3403,7 @@
         <v>0.00184185349580253</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>500</v>
       </c>
@@ -2903,7 +3431,7 @@
         <v>0.00131445855773394</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>1000</v>
       </c>
@@ -2931,16 +3459,16 @@
         <v>0.00667392607840393</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3" t="s">
         <v>2</v>
       </c>
@@ -2963,7 +3491,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>1</v>
       </c>
@@ -2988,10 +3516,10 @@
       </c>
       <c r="H14" s="0" t="n">
         <f aca="false">STDEV(B14:F14)</f>
-        <v>0.00332553149135594</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.00332553149135592</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>10</v>
       </c>
@@ -3019,7 +3547,7 @@
         <v>0.0630254781473334</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>50</v>
       </c>
@@ -3047,7 +3575,7 @@
         <v>0.161644744183967</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>100</v>
       </c>
@@ -3072,10 +3600,10 @@
       </c>
       <c r="H17" s="0" t="n">
         <f aca="false">STDEV(B17:F17)</f>
-        <v>0.0585407183317731</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.0585407183317732</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>200</v>
       </c>
@@ -3103,7 +3631,7 @@
         <v>0.00162069630097684</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>250</v>
       </c>
@@ -3131,7 +3659,7 @@
         <v>0.00341594427647759</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>500</v>
       </c>
@@ -3159,7 +3687,7 @@
         <v>0.00137650524880946</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>1000</v>
       </c>
@@ -3187,16 +3715,16 @@
         <v>0.00172718041906455</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="3" t="s">
         <v>2</v>
       </c>
@@ -3219,7 +3747,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>1</v>
       </c>
@@ -3247,7 +3775,7 @@
         <v>0.00457257074302848</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>10</v>
       </c>
@@ -3275,7 +3803,7 @@
         <v>0.128864860448844</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>50</v>
       </c>
@@ -3303,7 +3831,7 @@
         <v>0.355656272698374</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>100</v>
       </c>
@@ -3331,7 +3859,7 @@
         <v>0.0498100576761361</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>200</v>
       </c>
@@ -3359,7 +3887,7 @@
         <v>0.0743308865963537</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>250</v>
       </c>
@@ -3387,7 +3915,7 @@
         <v>0.258251502650614</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>500</v>
       </c>
@@ -3415,7 +3943,7 @@
         <v>0.0388909811678749</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>1000</v>
       </c>
@@ -3443,19 +3971,19 @@
         <v>0.00800971511977798</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -3464,13 +3992,12 @@
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B23:F23"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>